<commit_message>
added job posting data
</commit_message>
<xml_diff>
--- a/Linkedin_URLs_Company_List_POC.xlsx
+++ b/Linkedin_URLs_Company_List_POC.xlsx
@@ -82,7 +82,7 @@
     <t xml:space="preserve">HCA</t>
   </si>
   <si>
-    <t xml:space="preserve">LEMONADE, INC.  | LinkedIn</t>
+    <t xml:space="preserve">LEMONADE  | LinkedIn</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.linkedin.com/company/lemonade-inc-/</t>
@@ -330,13 +330,13 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="68.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="68.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.57"/>
   </cols>
   <sheetData>

</xml_diff>